<commit_message>
REPORT COMMIT: Mon 13/11/2017_23:13:46.00
</commit_message>
<xml_diff>
--- a/Pugh_Matrix_Motor.xlsx
+++ b/Pugh_Matrix_Motor.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
   <si>
     <t>Quality</t>
   </si>
@@ -145,6 +145,162 @@
   </si>
   <si>
     <t>Level of Knowledge Required</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Module Type:</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>Filename:</t>
+  </si>
+  <si>
+    <t>Circular Buffer </t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Impliments a fixed-size buffer data structure for use in buffering our command data stream in the UART module.</t>
+  </si>
+  <si>
+    <t>circ_buffer.c</t>
+  </si>
+  <si>
+    <t>Command Line Buffer</t>
+  </si>
+  <si>
+    <t>Impliments the Buffer to be used in the Command Parser module</t>
+  </si>
+  <si>
+    <t>cmd_line_buffer.c</t>
+  </si>
+  <si>
+    <t>Command Parser</t>
+  </si>
+  <si>
+    <t>Handles Input received from UART in the Main module</t>
+  </si>
+  <si>
+    <t>cmd_parser.c</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Calculates our Linearised Controller to be executed in the Main module</t>
+  </si>
+  <si>
+    <t>controller.c</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Handles Encoder input</t>
+  </si>
+  <si>
+    <t>encoder.c</t>
+  </si>
+  <si>
+    <t>Encoder Interrupt Service Routine</t>
+  </si>
+  <si>
+    <t>Handles Encoder ISRs</t>
+  </si>
+  <si>
+    <t>encoder_isr.c</t>
+  </si>
+  <si>
+    <t>Log Data</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Outputs requested Logged Data to console</t>
+  </si>
+  <si>
+    <t>log_data.c</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>The core program that runs on startup</t>
+  </si>
+  <si>
+    <t>main.c</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Handles Potentiometer input</t>
+  </si>
+  <si>
+    <t>potentiometer.c</t>
+  </si>
+  <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>Reserved for Startup self-checks, initialisation routines and serial handshake</t>
+  </si>
+  <si>
+    <t>Startup.c</t>
+  </si>
+  <si>
+    <t>Stepper</t>
+  </si>
+  <si>
+    <t>Handles Stepper Output</t>
+  </si>
+  <si>
+    <t>stepper.c</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Establishes a 100Hz Loop for time-critical tasks</t>
+  </si>
+  <si>
+    <t>task.c</t>
+  </si>
+  <si>
+    <t>Task Interrupt Service Routine</t>
+  </si>
+  <si>
+    <t>Handles Task ISRs</t>
+  </si>
+  <si>
+    <t>task_isr.c</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Handles UART communications</t>
+  </si>
+  <si>
+    <t>uart.c</t>
+  </si>
+  <si>
+    <t>UART Interrupt Service Routine</t>
+  </si>
+  <si>
+    <t>Handles UART ISRs</t>
+  </si>
+  <si>
+    <t>uart_isr.c</t>
   </si>
 </sst>
 </file>
@@ -154,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +347,12 @@
       <color rgb="FFE7EDF0"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFE7EDF0"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -212,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -553,11 +715,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF3E6F89"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF3E6F89"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC5D3DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC5D3DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF3E6F89"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF3E6F89"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF3E6F89"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF3E6F89"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF3E6F89"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,6 +821,39 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -628,33 +869,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -668,6 +882,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1844,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20376B-42D1-47C6-B00E-3423DC71A09B}">
-  <dimension ref="B1:U41"/>
+  <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="H39" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1861,6 +2099,10 @@
     <col min="15" max="16" width="16.6328125" customWidth="1"/>
     <col min="18" max="18" width="18.6328125" customWidth="1"/>
     <col min="19" max="21" width="4.6328125" customWidth="1"/>
+    <col min="25" max="25" width="16.6328125" customWidth="1"/>
+    <col min="26" max="26" width="12.6328125" customWidth="1"/>
+    <col min="27" max="27" width="24.6328125" customWidth="1"/>
+    <col min="28" max="28" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -1872,14 +2114,14 @@
       <c r="E1" s="28"/>
       <c r="F1" s="1"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
       <c r="N1" s="18"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -1944,13 +2186,13 @@
       <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
@@ -2257,25 +2499,25 @@
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="2:21" ht="4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="34"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="25"/>
     </row>
     <row r="12" spans="2:21" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
@@ -2323,10 +2565,10 @@
     </row>
     <row r="17" spans="15:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="15:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="O18" s="24" t="s">
+      <c r="O18" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="P18" s="25"/>
+      <c r="P18" s="36"/>
     </row>
     <row r="19" spans="15:16" ht="4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="O19" s="8"/>
@@ -2415,8 +2657,8 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="2:28" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="26" t="s">
         <v>32</v>
       </c>
@@ -2424,7 +2666,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="28"/>
     </row>
-    <row r="35" spans="2:5" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="12" t="s">
         <v>33</v>
@@ -2436,13 +2678,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" ht="4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="29"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
       <c r="E36" s="31"/>
     </row>
-    <row r="37" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
@@ -2454,7 +2696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
@@ -2466,7 +2708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
         <v>38</v>
       </c>
@@ -2478,7 +2720,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="2:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="6" t="s">
         <v>39</v>
       </c>
@@ -2490,11 +2732,248 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="32"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
+    <row r="41" spans="2:28" ht="4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="43" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y44" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z44" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA44" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB44" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" ht="4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="43"/>
+      <c r="AA45" s="43"/>
+      <c r="AB45" s="44"/>
+    </row>
+    <row r="46" spans="2:28" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y46" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z46" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA46" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB46" s="45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y47" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z47" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA47" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB47" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y48" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z48" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA48" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB48" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="25:28" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y49" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z49" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA49" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB49" s="45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="25:28" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y50" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z50" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA50" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB50" s="45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z51" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA51" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB51" s="45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y52" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z52" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA52" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB52" s="45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y53" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z53" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA53" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB53" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="25:28" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y54" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z54" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA54" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB54" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="25:28" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y55" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z55" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA55" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB55" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="25:28" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y56" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z56" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA56" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB56" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y57" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z57" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA57" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB57" s="45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y58" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z58" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA58" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB58" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y59" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z59" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA59" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB59" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="25:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y60" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z60" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA60" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB60" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="25:28" ht="4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y61" s="46"/>
+      <c r="Z61" s="47"/>
+      <c r="AA61" s="47"/>
+      <c r="AB61" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>